<commit_message>
augmented data sequence class
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="111">
   <si>
     <t>No</t>
   </si>
@@ -318,9 +318,6 @@
   </si>
   <si>
     <t>Add horizontal flip</t>
-  </si>
-  <si>
-    <t>~Krizhevsky architecture</t>
   </si>
   <si>
     <t>model_v19.h5</t>
@@ -502,19 +499,48 @@
     <t>42sec</t>
   </si>
   <si>
-    <t>Top 5: 99.8 and 69.7</t>
-  </si>
-  <si>
     <t>99sec</t>
   </si>
   <si>
-    <t>Top 5: 94.1 and 39.1. Down by a lot</t>
-  </si>
-  <si>
     <t>80sec</t>
   </si>
   <si>
-    <t>Top 5: 22.3 and 22.2. Down by even more</t>
+    <t>86sec</t>
+  </si>
+  <si>
+    <t>Top 5: 33.2 and 31.0.</t>
+  </si>
+  <si>
+    <t>52sec</t>
+  </si>
+  <si>
+    <t>Top 5: 99.8 and 69.7. Down, maybe because dropout became after L3, not after L2?</t>
+  </si>
+  <si>
+    <t>Top 5: 94.1 and 39.1. Down by a lot. Perhaps too big jump D1_4096--&gt;D2_20 ?</t>
+  </si>
+  <si>
+    <t>Top 5: 22.3 and 22.2. Down by even more. Perhaps because droput became after L4, not L3?</t>
+  </si>
+  <si>
+    <t>~Krizhevsky architecture. Top 5: 79.0 and 72.4. Good improvement on variance!</t>
+  </si>
+  <si>
+    <t>Remove dropouts after CNN layers</t>
+  </si>
+  <si>
+    <t>51sec</t>
+  </si>
+  <si>
+    <t>By reading Kryzhevski paper, no dropout applied on conv layers. https://www.nvidia.cn/content/tesla/pdf/machine-learning/imagenet-classification-with-deep-convolutional-nn.pdf)
+Actual:  dropout on conv layers helps to not overfit</t>
+  </si>
+  <si>
+    <t>Reduce last dense layer 4096--&gt;128 (br.of v35)</t>
+  </si>
+  <si>
+    <t>As a result of degrading in v31==&gt;v32, decided to try reducing last dense layer
+Actual: test accuracy degraded</t>
   </si>
 </sst>
 </file>
@@ -565,7 +591,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -573,24 +599,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -906,87 +952,88 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N47"/>
+  <dimension ref="A1:N50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="E40" sqref="E40"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.28515625" customWidth="1"/>
-    <col min="3" max="4" width="4.28515625" customWidth="1"/>
-    <col min="5" max="5" width="50.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="3.28515625" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" customWidth="1"/>
-    <col min="8" max="8" width="9.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" customWidth="1"/>
-    <col min="11" max="11" width="87.140625" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" style="5" customWidth="1"/>
+    <col min="3" max="4" width="4.28515625" style="5" customWidth="1"/>
+    <col min="5" max="5" width="50.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.28515625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="5" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="5" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" style="5" customWidth="1"/>
+    <col min="10" max="10" width="11.140625" style="5" customWidth="1"/>
+    <col min="11" max="11" width="87.140625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="9.42578125" style="5" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>44</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="5">
         <v>50</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="5">
         <v>31.1</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="5">
         <v>26.7</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" customFormat="1" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="F3" t="s">
@@ -1005,11 +1052,11 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" customFormat="1" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="2" t="s">
         <v>13</v>
       </c>
       <c r="F4" t="s">
@@ -1026,71 +1073,71 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="A5" s="7">
         <v>43333</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5">
+      <c r="B5" s="7"/>
+      <c r="C5" s="5">
         <v>1</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="5">
         <v>50</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="5">
         <v>98.5</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="5">
         <v>17</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="K5" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="A6" s="7">
         <v>43334</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6">
+      <c r="B6" s="7"/>
+      <c r="C6" s="5">
         <v>2</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F6" t="s">
+      <c r="F6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="5">
         <v>50</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="5">
         <v>98.5</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="5">
         <v>26.2</v>
       </c>
-      <c r="K6" t="s">
+      <c r="K6" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
+    <row r="7" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
         <v>43334</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="1"/>
       <c r="C7">
         <v>3</v>
       </c>
       <c r="D7" t="s">
         <v>45</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F7" t="s">
@@ -1109,18 +1156,18 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:12" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
         <v>43335</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="1"/>
       <c r="C8">
         <v>4</v>
       </c>
       <c r="D8" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="2" t="s">
         <v>21</v>
       </c>
       <c r="F8" t="s">
@@ -1140,764 +1187,843 @@
       </c>
     </row>
     <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+      <c r="A9" s="7">
         <v>43336</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="5">
         <v>5</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="5">
         <v>50</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="5">
         <v>38.200000000000003</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K9" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+      <c r="A10" s="7">
         <v>43336</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="5">
         <v>6</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F10" t="s">
+      <c r="F10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="5">
         <v>100</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="5">
         <v>40.5</v>
       </c>
-      <c r="K10" t="s">
+      <c r="K10" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
+      <c r="A11" s="7">
         <v>43336</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="5">
         <v>7</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="5">
         <v>150</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="5">
         <v>41.4</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="5" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
+      <c r="A12" s="7">
         <v>43336</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="5">
         <v>8</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="5">
         <v>200</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="5">
         <v>46.7</v>
       </c>
-      <c r="J12">
+      <c r="J12" s="5">
         <v>38.200000000000003</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L12" t="s">
+      <c r="L12" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+      <c r="A13" s="7">
         <v>43349</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="5">
         <v>9</v>
       </c>
-      <c r="E13" s="5" t="s">
+      <c r="E13" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F13" t="s">
+      <c r="F13" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="5">
         <v>250</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="5">
         <v>48.3</v>
       </c>
-      <c r="J13">
+      <c r="J13" s="5">
         <v>39.299999999999997</v>
       </c>
-      <c r="K13" s="3" t="s">
+      <c r="K13" s="8" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+      <c r="A14" s="7">
         <v>43349</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="5">
         <v>10</v>
       </c>
-      <c r="E14" s="5" t="s">
+      <c r="E14" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="5">
         <v>450</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="5">
         <v>49.7</v>
       </c>
-      <c r="J14">
+      <c r="J14" s="5">
         <v>39.1</v>
       </c>
-      <c r="K14" t="s">
+      <c r="K14" s="5" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="A15" s="7">
         <v>43350</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="5">
         <v>11</v>
       </c>
-      <c r="E15" s="5" t="s">
+      <c r="E15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F15" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="5">
         <v>500</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="5">
         <v>52.7</v>
       </c>
-      <c r="J15">
+      <c r="J15" s="5">
         <v>39.799999999999997</v>
       </c>
-      <c r="K15" t="s">
+      <c r="K15" s="5" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="A16" s="7">
         <v>43354</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="5">
         <v>12</v>
       </c>
-      <c r="E16" s="5" t="s">
+      <c r="E16" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="F16" t="s">
+      <c r="F16" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="5">
         <v>50</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="5">
         <v>98.4</v>
       </c>
-      <c r="J16">
+      <c r="J16" s="5">
         <v>16.600000000000001</v>
       </c>
-      <c r="K16" t="s">
+      <c r="K16" s="5" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="60" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="A17" s="7">
         <v>43355</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="5">
         <v>13</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E17" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="5">
         <v>128</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="5">
         <v>81.900000000000006</v>
       </c>
-      <c r="J17">
+      <c r="J17" s="5">
         <v>24.2</v>
       </c>
-      <c r="K17" s="3" t="s">
+      <c r="K17" s="8" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="A18" s="7">
         <v>43356</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="5">
         <v>14</v>
       </c>
-      <c r="E18" s="5" t="s">
+      <c r="E18" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="F18" t="s">
+      <c r="F18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="5">
         <v>192</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="5">
         <v>83.8</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="5">
         <v>24.8</v>
       </c>
-      <c r="K18" s="3" t="s">
+      <c r="K18" s="8" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="A19" s="7">
         <v>43357</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="5">
         <v>15</v>
       </c>
-      <c r="E19" s="5" t="s">
+      <c r="E19" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="5">
         <f>192+144</f>
         <v>336</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="5">
         <v>86.3</v>
       </c>
-      <c r="J19">
+      <c r="J19" s="5">
         <v>25.2</v>
       </c>
-      <c r="K19" s="3" t="s">
+      <c r="K19" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19" s="5" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="A20" s="7">
         <v>43357</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="5">
         <v>16</v>
       </c>
-      <c r="E20" s="5" t="s">
+      <c r="E20" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F20" t="s">
+      <c r="F20" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="5">
         <v>64</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="5">
         <v>69.400000000000006</v>
       </c>
-      <c r="J20">
+      <c r="J20" s="5">
         <v>30.1</v>
       </c>
-      <c r="K20" s="3" t="s">
+      <c r="K20" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="L20" t="s">
+      <c r="L20" s="5" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="A21" s="7">
         <v>43358</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="5">
         <v>17</v>
       </c>
-      <c r="E21" s="5" t="s">
+      <c r="E21" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="5">
         <f>H20+64*3</f>
         <v>256</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="5">
         <v>78.8</v>
       </c>
-      <c r="J21">
+      <c r="J21" s="5">
         <v>28.1</v>
       </c>
-      <c r="K21" s="3" t="s">
+      <c r="K21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="L21" t="s">
+      <c r="L21" s="5" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="A22" s="7">
         <v>43360</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="5">
         <v>18</v>
       </c>
-      <c r="E22" s="5" t="s">
+      <c r="E22" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="5">
         <f>H21+144</f>
         <v>400</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="5">
         <v>71.400000000000006</v>
       </c>
-      <c r="J22">
+      <c r="J22" s="5">
         <v>31</v>
       </c>
-      <c r="K22" s="3" t="s">
+      <c r="K22" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="L22" t="s">
+      <c r="L22" s="5" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="A23" s="7">
         <v>43383</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C23" s="5">
+        <v>19</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="G23" s="5">
+        <v>10</v>
+      </c>
+      <c r="H23" s="5">
+        <v>1840</v>
+      </c>
+      <c r="I23" s="5">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="J23" s="5">
+        <v>28.4</v>
+      </c>
+      <c r="K23" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="L23" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="N23" s="5" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="7">
+        <v>43384</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C23">
-        <v>19</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="G23">
-        <v>10</v>
-      </c>
-      <c r="H23">
-        <v>1840</v>
-      </c>
-      <c r="I23">
-        <v>66.599999999999994</v>
-      </c>
-      <c r="J23">
-        <v>28.4</v>
-      </c>
-      <c r="K23" s="3" t="s">
+      <c r="C24" s="5">
+        <v>20</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="G24" s="5">
+        <v>5</v>
+      </c>
+      <c r="H24" s="5">
+        <v>720</v>
+      </c>
+      <c r="I24" s="5">
+        <v>65.8</v>
+      </c>
+      <c r="J24" s="5">
+        <v>26.9</v>
+      </c>
+      <c r="K24" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="L23" t="s">
-        <v>75</v>
-      </c>
-      <c r="N23" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+      <c r="N24" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="7">
         <v>43384</v>
       </c>
-      <c r="B24" t="s">
-        <v>83</v>
-      </c>
-      <c r="C24">
-        <v>20</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G24">
-        <v>5</v>
-      </c>
-      <c r="H24">
-        <v>720</v>
-      </c>
-      <c r="I24">
-        <v>65.8</v>
-      </c>
-      <c r="J24">
-        <v>26.9</v>
-      </c>
-      <c r="K24" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="N24" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>43384</v>
-      </c>
-      <c r="C25">
+      <c r="C25" s="5">
         <v>21</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="E25" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="5">
         <v>1</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="5">
         <v>256</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="5">
         <v>5.6</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="5">
         <v>4.5999999999999996</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>91</v>
+      <c r="K25" s="8" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
+      <c r="A26" s="7">
         <v>43385</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="5">
         <v>23</v>
       </c>
-      <c r="E26" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="G26">
+      <c r="E26" s="6" t="s">
+        <v>89</v>
+      </c>
+      <c r="G26" s="5">
         <v>3</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="5">
         <f>144*G26</f>
         <v>432</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="5">
         <v>40.200000000000003</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="5">
         <v>17.3</v>
       </c>
-      <c r="K26" s="3" t="s">
+      <c r="K26" s="8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A27" s="7"/>
+      <c r="E27" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
+      <c r="E28" s="6" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A29" s="7">
+        <v>43385</v>
+      </c>
+      <c r="C29" s="5">
+        <v>26</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G29" s="5">
+        <v>2</v>
+      </c>
+      <c r="H29" s="5">
+        <v>288</v>
+      </c>
+      <c r="I29" s="5">
+        <v>80.8</v>
+      </c>
+      <c r="J29" s="5">
+        <v>28.6</v>
+      </c>
+      <c r="K29" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="N29" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="E27" s="5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="E28" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A30" s="7"/>
+      <c r="E30" s="6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A31" s="7"/>
+      <c r="E31" s="6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
+      <c r="E32" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A33" s="7">
         <v>43385</v>
       </c>
-      <c r="C29">
-        <v>26</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="G29">
-        <v>2</v>
-      </c>
-      <c r="H29">
-        <v>288</v>
-      </c>
-      <c r="I29">
-        <v>80.8</v>
-      </c>
-      <c r="J29">
-        <v>28.6</v>
-      </c>
-      <c r="K29" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="N29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="E30" s="5" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="E31" s="5" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="E32" s="5" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
-        <v>43385</v>
-      </c>
-      <c r="C33">
+      <c r="C33" s="5">
         <v>30</v>
       </c>
-      <c r="E33" s="5" t="s">
+      <c r="E33" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="5">
         <v>3</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="5">
         <f>144*3</f>
         <v>432</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="5">
         <v>97.8</v>
       </c>
-      <c r="J33" s="6">
+      <c r="J33" s="9">
         <v>32.700000000000003</v>
       </c>
-      <c r="K33" t="s">
-        <v>96</v>
-      </c>
-      <c r="N33" t="s">
+      <c r="K33" s="5" t="s">
         <v>95</v>
       </c>
+      <c r="N33" s="5" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="A34" s="7">
         <v>43386</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="5">
         <v>31</v>
       </c>
-      <c r="E34" s="5" t="s">
+      <c r="E34" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="5">
         <v>3</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="5">
         <f t="shared" ref="H34:H39" si="0">144*3</f>
         <v>432</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="5">
         <v>95.2</v>
       </c>
-      <c r="J34">
+      <c r="J34" s="5">
         <v>30.6</v>
       </c>
-      <c r="K34" t="s">
-        <v>98</v>
-      </c>
-      <c r="N34" t="s">
-        <v>97</v>
+      <c r="K34" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="N34" s="5" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="A35" s="7">
         <v>43387</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="5">
         <v>32</v>
       </c>
-      <c r="E35" s="5" t="s">
+      <c r="E35" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="5">
         <v>3</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="5">
         <f t="shared" si="0"/>
         <v>432</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="5">
         <v>91.6</v>
       </c>
-      <c r="J35">
+      <c r="J35" s="5">
         <v>22</v>
       </c>
-      <c r="K35" t="s">
-        <v>100</v>
-      </c>
-      <c r="N35" t="s">
-        <v>99</v>
+      <c r="K35" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="N35" s="5" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A36" s="2">
+      <c r="A36" s="7">
         <v>43388</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="5">
         <v>33</v>
       </c>
-      <c r="E36" s="5" t="s">
+      <c r="E36" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="5">
         <v>3</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="5">
         <f t="shared" si="0"/>
         <v>432</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="5">
         <v>7</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="5">
         <v>6.1</v>
       </c>
-      <c r="K36" t="s">
-        <v>102</v>
-      </c>
-      <c r="N36" t="s">
-        <v>101</v>
+      <c r="K36" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A37" s="2">
-        <v>43389</v>
-      </c>
-      <c r="C37">
+      <c r="A37" s="7">
+        <v>43388</v>
+      </c>
+      <c r="C37" s="5">
         <v>34</v>
       </c>
-      <c r="E37" s="5" t="s">
+      <c r="E37" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="5">
         <v>3</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="5">
         <f t="shared" si="0"/>
         <v>432</v>
       </c>
+      <c r="I37" s="5">
+        <v>7.2</v>
+      </c>
+      <c r="J37" s="5">
+        <v>6.7</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="N37" s="5" t="s">
+        <v>99</v>
+      </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A38" s="2"/>
-      <c r="E38" s="5" t="s">
+      <c r="A38" s="7"/>
+      <c r="E38" s="6" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
-        <v>43390</v>
-      </c>
-      <c r="C39">
-        <v>36</v>
-      </c>
-      <c r="E39" s="5" t="s">
+      <c r="A39" s="7">
+        <v>43389</v>
+      </c>
+      <c r="C39" s="5">
+        <v>35</v>
+      </c>
+      <c r="E39" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="5">
         <v>3</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="5">
         <f t="shared" si="0"/>
         <v>432</v>
       </c>
-      <c r="K39" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E40" s="5" t="s">
+      <c r="I39" s="5">
+        <v>36.799999999999997</v>
+      </c>
+      <c r="J39" s="5">
+        <v>30.6</v>
+      </c>
+      <c r="K39" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="N39" s="5" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="7">
+        <v>43389</v>
+      </c>
+      <c r="C40" s="5">
+        <v>36</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G40" s="5">
+        <v>1</v>
+      </c>
+      <c r="H40" s="5">
+        <v>144</v>
+      </c>
+      <c r="I40" s="5">
+        <v>48.7</v>
+      </c>
+      <c r="J40" s="5">
+        <v>27.9</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="N40" s="5" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="7">
+        <v>43389</v>
+      </c>
+      <c r="C41" s="5">
+        <v>37</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="G41" s="5">
+        <v>1</v>
+      </c>
+      <c r="H41" s="5">
+        <v>144</v>
+      </c>
+      <c r="I41" s="5">
+        <v>50.6</v>
+      </c>
+      <c r="J41" s="5">
+        <v>28.2</v>
+      </c>
+      <c r="K41" s="8" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A42" s="7"/>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E43" s="6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E44" s="6" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E46" s="6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E47" s="6" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E41" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E43" s="5" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E44" s="5" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E45" s="5" t="s">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="E48" s="6" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E46" s="5" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E47" s="5" t="s">
-        <v>77</v>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E49" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E50" s="6" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
random crops + hor flip for training 4 corners + center for testing
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="134">
   <si>
     <t>No</t>
   </si>
@@ -316,9 +316,6 @@
     <t>Crops 12=&gt;16</t>
   </si>
   <si>
-    <t>Add horizontal flip</t>
-  </si>
-  <si>
     <t>model_v19.h5</t>
   </si>
   <si>
@@ -326,9 +323,6 @@
   </si>
   <si>
     <t>contrast normalization</t>
-  </si>
-  <si>
-    <t>inception again</t>
   </si>
   <si>
     <t>#18 keep training for 10 full epochs (10x144 passes through data). Changed batch size to 64</t>
@@ -578,6 +572,9 @@
     <t>model_v39.h5</t>
   </si>
   <si>
+    <t>data squarized (cut longer dim)</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">Top 5: 100.0 and </t>
     </r>
@@ -602,17 +599,118 @@
         <scheme val="minor"/>
       </rPr>
       <t>No diff in speed on SSD and HDD except 1 iteration
-High spikes on GPU - try reducing/squarizing images from ilsvrc
-55 sec/epoch; vs. 22sec on non-ilsvrc data
+High spikes on GPU - try reducing/squarizing images from ilsvrc (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>worked as expected after squarizing- did not reduce</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
+55 sec/epoch; vs. 22sec on non-ilsvrc data (</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>become 36sec after squarizing, which is proportional to number of images in dataset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)
 Huge improvement on test test - looks like dataset is better than my donwloaded from google. try visualizing interim layers</t>
     </r>
+  </si>
+  <si>
+    <t>paralell data loading</t>
+  </si>
+  <si>
+    <t>run time to process 100 batches decreased 38==&gt;36sec. To load each batch takes ~0.35sec (so it's on critical path)</t>
+  </si>
+  <si>
+    <t>224/256 crops, randomly chosen</t>
+  </si>
+  <si>
+    <t>224/256 crops + hor_flip, randomly chosen</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Top5: 99.7 and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>92.6</t>
+    </r>
+  </si>
+  <si>
+    <t>Evaluate on 5 frames (4 corners + center)</t>
+  </si>
+  <si>
+    <t>Looks like need longer training</t>
+  </si>
+  <si>
+    <t>train longer</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Top5: 98.4 and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>92.5</t>
+    </r>
+  </si>
+  <si>
+    <t>1 frame=&gt;5 frames: test accuracy 60.7--&gt;63.4 (top 5 test: 90.9--&gt;91.8). Use it!</t>
+  </si>
+  <si>
+    <t>Evaluate on 10 frames (add hor flip)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -648,6 +746,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -690,7 +796,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -709,6 +815,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1024,10 +1131,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N55"/>
+  <dimension ref="A1:N62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="K49" sqref="K49"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E59" sqref="E59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,7 +1173,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>6</v>
@@ -1645,13 +1752,13 @@
         <v>43383</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C23" s="5">
         <v>19</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G23" s="5">
         <v>10</v>
@@ -1666,13 +1773,13 @@
         <v>28.4</v>
       </c>
       <c r="K23" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L23" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N23" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="45" x14ac:dyDescent="0.25">
@@ -1680,7 +1787,7 @@
         <v>43384</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C24" s="5">
         <v>20</v>
@@ -1701,10 +1808,10 @@
         <v>26.9</v>
       </c>
       <c r="K24" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="N24" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -1730,7 +1837,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="K25" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
@@ -1741,7 +1848,7 @@
         <v>23</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G26" s="5">
         <v>3</v>
@@ -1757,7 +1864,7 @@
         <v>17.3</v>
       </c>
       <c r="K26" s="8" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
@@ -1795,10 +1902,10 @@
         <v>28.6</v>
       </c>
       <c r="K29" s="8" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="N29" s="5" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
@@ -1843,10 +1950,10 @@
         <v>32.700000000000003</v>
       </c>
       <c r="K33" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="N33" s="5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
@@ -1873,10 +1980,10 @@
         <v>30.6</v>
       </c>
       <c r="K34" s="5" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="N34" s="5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
@@ -1903,10 +2010,10 @@
         <v>22</v>
       </c>
       <c r="K35" s="5" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="N35" s="5" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
@@ -1933,10 +2040,10 @@
         <v>6.1</v>
       </c>
       <c r="K36" s="5" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="N36" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
@@ -1963,10 +2070,10 @@
         <v>6.7</v>
       </c>
       <c r="K37" s="5" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="N37" s="5" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
@@ -1999,10 +2106,10 @@
         <v>30.6</v>
       </c>
       <c r="K39" s="5" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N39" s="5" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="40" spans="1:14" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2013,7 +2120,7 @@
         <v>36</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G40" s="5">
         <v>1</v>
@@ -2028,10 +2135,10 @@
         <v>27.9</v>
       </c>
       <c r="K40" s="8" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="N40" s="5" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:14" ht="30" x14ac:dyDescent="0.25">
@@ -2042,7 +2149,7 @@
         <v>37</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="G41" s="5">
         <v>1</v>
@@ -2057,7 +2164,7 @@
         <v>28.2</v>
       </c>
       <c r="K41" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
@@ -2068,7 +2175,7 @@
         <v>38</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="G42" s="5">
         <v>1</v>
@@ -2083,7 +2190,7 @@
         <v>30.9</v>
       </c>
       <c r="K42" s="5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
@@ -2091,7 +2198,7 @@
         <v>43391</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G43" s="5">
         <v>10</v>
@@ -2106,7 +2213,7 @@
         <v>27.1</v>
       </c>
       <c r="K43" s="5" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
@@ -2117,7 +2224,7 @@
         <v>39</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="G44" s="5">
         <v>50</v>
@@ -2132,13 +2239,13 @@
         <v>33.6</v>
       </c>
       <c r="L44" s="5" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="E45" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G45" s="5">
         <v>100</v>
@@ -2153,13 +2260,13 @@
         <v>32.5</v>
       </c>
       <c r="K45" s="5" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="E46" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G46" s="5">
         <v>150</v>
@@ -2174,13 +2281,13 @@
         <v>32.700000000000003</v>
       </c>
       <c r="K46" s="5" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="E47" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G47" s="5">
         <v>100</v>
@@ -2195,10 +2302,10 @@
         <v>33.200000000000003</v>
       </c>
       <c r="K47" s="5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>43392</v>
       </c>
@@ -2206,7 +2313,7 @@
         <v>40</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G48" s="5">
         <v>50</v>
@@ -2221,40 +2328,176 @@
         <v>62</v>
       </c>
       <c r="K48" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="L48" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A49" s="7">
+        <v>43397</v>
+      </c>
+      <c r="E49" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="G49" s="5">
+        <v>50</v>
+      </c>
+      <c r="H49" s="5">
+        <v>50</v>
+      </c>
+      <c r="I49" s="5">
+        <v>94.9</v>
+      </c>
+      <c r="J49" s="10">
+        <v>58.6</v>
+      </c>
+      <c r="K49" s="8"/>
+    </row>
+    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="7">
+        <v>43397</v>
+      </c>
+      <c r="C50" s="5">
+        <v>41</v>
+      </c>
+      <c r="E50" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="L48" s="5" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="50" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E50" s="6" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="51" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="G50" s="5">
+        <v>50</v>
+      </c>
+      <c r="H50" s="5">
+        <v>50</v>
+      </c>
+      <c r="J50" s="9"/>
+      <c r="K50" s="8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <v>43398</v>
+      </c>
       <c r="E51" s="6" t="s">
+        <v>125</v>
+      </c>
+      <c r="G51" s="5">
+        <v>50</v>
+      </c>
+      <c r="H51" s="5">
+        <v>50</v>
+      </c>
+      <c r="I51" s="5">
+        <v>89.6</v>
+      </c>
+      <c r="J51" s="9">
+        <v>65.3</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <v>43398</v>
+      </c>
+      <c r="C52" s="5">
+        <v>42</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>126</v>
+      </c>
+      <c r="G52" s="5">
+        <v>50</v>
+      </c>
+      <c r="H52" s="5">
+        <v>50</v>
+      </c>
+      <c r="I52" s="5">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="J52" s="10">
+        <v>62.7</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A53" s="7">
+        <v>43398</v>
+      </c>
+      <c r="E53" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="I53" s="5">
+        <v>80.8</v>
+      </c>
+      <c r="J53" s="9">
+        <v>63.6</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A54" s="7">
+        <v>43398</v>
+      </c>
+      <c r="C54" s="5">
+        <v>43</v>
+      </c>
+      <c r="E54" s="6" t="s">
+        <v>130</v>
+      </c>
+      <c r="G54" s="5">
+        <v>100</v>
+      </c>
+      <c r="H54" s="5">
+        <v>100</v>
+      </c>
+      <c r="I54" s="5">
+        <v>83.8</v>
+      </c>
+      <c r="J54" s="9">
+        <v>63.4</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A55" s="7">
+        <v>43399</v>
+      </c>
+      <c r="C55" s="5">
+        <v>44</v>
+      </c>
+      <c r="E55" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="J55" s="9"/>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E59" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E52" s="6" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="53" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E53" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="54" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E54" s="6" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="55" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E55" s="6" t="s">
-        <v>76</v>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E60" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E61" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E62" s="6" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
early stopping evaluation on 5==>10 frames
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="136">
   <si>
     <t>No</t>
   </si>
@@ -703,20 +703,78 @@
     <t>1 frame=&gt;5 frames: test accuracy 60.7--&gt;63.4 (top 5 test: 90.9--&gt;91.8). Use it!</t>
   </si>
   <si>
-    <t>Evaluate on 10 frames (add hor flip)</t>
+    <t>Early stopping (1% validation accuracy improvement, patience= epochs)</t>
+  </si>
+  <si>
+    <t>Evaluate on 10 frames (add hor flip). Change early stopping criteria to 0.1% and 10 epoch patience</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Validation  top 1 accuracy on 1,5,10 frames: 54.4, 53.1, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>54.6</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Top 5 on 1, 5, 10 frames: 89.0, 90.0, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>90.4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. Marginal improvement</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="186"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -796,14 +854,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -814,7 +872,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -1131,10 +1190,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N62"/>
+  <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="E59" sqref="E59"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="K57" sqref="K57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1144,7 +1203,7 @@
     <col min="3" max="4" width="4.28515625" style="5" customWidth="1"/>
     <col min="5" max="5" width="50.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="3.28515625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="7.7109375" style="5" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="5" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" style="5" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" style="5" customWidth="1"/>
     <col min="10" max="10" width="11.140625" style="5" customWidth="1"/>
@@ -2468,7 +2527,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>43399</v>
       </c>
@@ -2478,25 +2537,50 @@
       <c r="E55" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="J55" s="9"/>
-    </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E59" s="6" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E60" s="6" t="s">
-        <v>78</v>
+      <c r="G55" s="5">
+        <v>24</v>
+      </c>
+      <c r="H55" s="5">
+        <v>24</v>
+      </c>
+      <c r="I55" s="5">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="J55" s="11">
+        <v>56.7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="7">
+        <v>43399</v>
+      </c>
+      <c r="E56" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="J56" s="5">
+        <v>54.6</v>
+      </c>
+      <c r="K56" s="8" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E61" s="6" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="E62" s="6" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E63" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="E64" s="6" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
reducing dropouts, 1st try to eliminate bias
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="147">
   <si>
     <t>No</t>
   </si>
@@ -777,10 +777,19 @@
     <t>Architecture to match Kryzvski: L1 filter size/stride 7/2==&gt;11/4</t>
   </si>
   <si>
-    <t>stopped training. Adam optimizer at fault. Diagnostics show 0.0 value gradients. Changing to SGD</t>
-  </si>
-  <si>
     <t>Adam to SGD (with 50 classes and full kryzkevski architecture, adam did not train)</t>
+  </si>
+  <si>
+    <t>Top 5: 86.6</t>
+  </si>
+  <si>
+    <t>did not converge while training. Adam optimizer at fault. Diagnostics show 0.0 value gradients. Changing to SGD</t>
+  </si>
+  <si>
+    <t>Remove dropouts (Trying to reduce bias). Early stopping val_acc --&gt; acc (temporarily)</t>
+  </si>
+  <si>
+    <t>Concl: architecture is big enough since bias is small. Now, need to work on variance</t>
   </si>
 </sst>
 </file>
@@ -887,7 +896,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -908,6 +917,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1223,10 +1233,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N65"/>
+  <dimension ref="A1:N71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="H60" sqref="H60"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="J62" sqref="J62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2653,6 +2663,9 @@
       <c r="E59" s="6" t="s">
         <v>141</v>
       </c>
+      <c r="H59" s="5">
+        <v>20</v>
+      </c>
       <c r="I59" s="5">
         <v>2</v>
       </c>
@@ -2660,7 +2673,7 @@
         <v>2</v>
       </c>
       <c r="K59" s="5" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -2671,31 +2684,87 @@
         <v>48</v>
       </c>
       <c r="E60" s="6" t="s">
+        <v>142</v>
+      </c>
+      <c r="H60" s="5">
+        <v>105</v>
+      </c>
+      <c r="I60" s="5">
+        <v>74.8</v>
+      </c>
+      <c r="J60" s="9">
+        <v>59.3</v>
+      </c>
+      <c r="K60" s="5" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="61" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="7">
+        <v>43426</v>
+      </c>
+      <c r="C61" s="5">
+        <v>49</v>
+      </c>
       <c r="E61" s="6" t="s">
+        <v>145</v>
+      </c>
+      <c r="I61" s="9">
+        <v>99.3</v>
+      </c>
+      <c r="J61" s="12">
+        <v>44.9</v>
+      </c>
+      <c r="K61" s="5" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A62" s="7"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="12"/>
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A63" s="7"/>
+      <c r="I63" s="9"/>
+      <c r="J63" s="12"/>
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="12"/>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A65" s="7"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="12"/>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A66" s="7"/>
+      <c r="J66" s="9"/>
+    </row>
+    <row r="67" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="E67" s="6" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E62" s="6" t="s">
+    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E68" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E63" s="6" t="s">
+    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E69" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E64" s="6" t="s">
+    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E70" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E65" s="6" t="s">
+    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="E71" s="6" t="s">
         <v>135</v>
       </c>
     </row>

</xml_diff>

<commit_message>
visualize false predictions; 50->100 classes
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$19</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="175">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="174">
   <si>
     <t>No</t>
   </si>
@@ -754,9 +754,6 @@
     <t>Change early stopping criteria to 0.1% and 20 epoch patience</t>
   </si>
   <si>
-    <t>PCA</t>
-  </si>
-  <si>
     <t>vgg- winner ilsvr'14 clsf:
 -
 -</t>
@@ -884,47 +881,61 @@
     <t>train longer (keep training prev model for 40 epochs)</t>
   </si>
   <si>
-    <t>Top 5: 87.0</t>
-  </si>
-  <si>
     <t>Top 5: 87.1. Same. 1 epoch time increases 98==&gt;127sec</t>
   </si>
   <si>
-    <t>Top 5: 87.2</t>
-  </si>
-  <si>
     <t>Increase PCA distortion's value: std 0.1=&gt;0.3. Keep training the same model  (keep training prev model for 40 epochs)</t>
   </si>
   <si>
     <t>Increase PCA distortion's value: std 0.3=&gt;1.0. Keep training the same model  (keep training prev model for 55 epochs)</t>
   </si>
   <si>
-    <t>Top 5: 87.9</t>
-  </si>
-  <si>
     <t>Increase PCA distortion's value: std 1.0=&gt;3.0. Keep training the same model  (keep training prev model for 51 epochs)</t>
   </si>
   <si>
-    <t>Top 5: 84.4</t>
-  </si>
-  <si>
     <t>PCA distortion's value: std 10.0. Train new</t>
   </si>
   <si>
     <t>PCA distortion's value: std 3.0. Train new</t>
+  </si>
+  <si>
+    <t>PCA distortion's value: std 1.0. Train new</t>
+  </si>
+  <si>
+    <t>Test top5 acc%</t>
+  </si>
+  <si>
+    <t>PCA distortion's value: std 0.3 Train new</t>
+  </si>
+  <si>
+    <t>50==&gt;100 classses</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="186"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1053,14 +1064,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1071,7 +1082,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1079,7 +1092,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1395,10 +1407,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:N82"/>
+  <dimension ref="A1:O86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E77" sqref="E77"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L79" sqref="L79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1411,13 +1424,13 @@
     <col min="7" max="7" width="7.7109375" style="5" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="9.85546875" style="5" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" style="5" customWidth="1"/>
-    <col min="10" max="10" width="11.140625" style="5" customWidth="1"/>
-    <col min="11" max="11" width="87.140625" style="5" customWidth="1"/>
-    <col min="12" max="12" width="9.42578125" style="5" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="5"/>
+    <col min="10" max="11" width="11.140625" style="5" customWidth="1"/>
+    <col min="12" max="12" width="87.140625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="9.42578125" style="5" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>16</v>
       </c>
@@ -1449,10 +1462,13 @@
         <v>4</v>
       </c>
       <c r="K1" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="E2" s="6" t="s">
         <v>2</v>
       </c>
@@ -1468,11 +1484,11 @@
       <c r="J2" s="5">
         <v>26.7</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:12" customFormat="1" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" customFormat="1" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D3" t="s">
         <v>45</v>
       </c>
@@ -1491,11 +1507,11 @@
       <c r="J3">
         <v>35.1</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:12" customFormat="1" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" customFormat="1" ht="32.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D4" t="s">
         <v>45</v>
       </c>
@@ -1515,7 +1531,7 @@
         <v>39.6</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="7">
         <v>43333</v>
       </c>
@@ -1538,11 +1554,11 @@
       <c r="J5" s="5">
         <v>17</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="L5" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>43334</v>
       </c>
@@ -1565,11 +1581,11 @@
       <c r="J6" s="5">
         <v>26.2</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:12" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43334</v>
       </c>
@@ -1595,11 +1611,11 @@
       <c r="J7">
         <v>35.700000000000003</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:12" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" customFormat="1" ht="16.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43335</v>
       </c>
@@ -1625,11 +1641,11 @@
       <c r="J8">
         <v>35</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="7">
         <v>43336</v>
       </c>
@@ -1651,11 +1667,11 @@
       <c r="I9" s="5">
         <v>38.200000000000003</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>43336</v>
       </c>
@@ -1677,11 +1693,11 @@
       <c r="I10" s="5">
         <v>40.5</v>
       </c>
-      <c r="K10" s="5" t="s">
+      <c r="L10" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="7">
         <v>43336</v>
       </c>
@@ -1703,11 +1719,11 @@
       <c r="I11" s="5">
         <v>41.4</v>
       </c>
-      <c r="K11" s="5" t="s">
+      <c r="L11" s="5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>43336</v>
       </c>
@@ -1732,14 +1748,14 @@
       <c r="J12" s="5">
         <v>38.200000000000003</v>
       </c>
-      <c r="K12" s="5" t="s">
+      <c r="L12" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="L12" s="5" t="s">
+      <c r="M12" s="5" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="13" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>43349</v>
       </c>
@@ -1764,11 +1780,11 @@
       <c r="J13" s="5">
         <v>39.299999999999997</v>
       </c>
-      <c r="K13" s="8" t="s">
+      <c r="L13" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>43349</v>
       </c>
@@ -1790,11 +1806,11 @@
       <c r="J14" s="5">
         <v>39.1</v>
       </c>
-      <c r="K14" s="5" t="s">
+      <c r="L14" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>43350</v>
       </c>
@@ -1816,11 +1832,11 @@
       <c r="J15" s="5">
         <v>39.799999999999997</v>
       </c>
-      <c r="K15" s="5" t="s">
+      <c r="L15" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>43354</v>
       </c>
@@ -1842,11 +1858,11 @@
       <c r="J16" s="5">
         <v>16.600000000000001</v>
       </c>
-      <c r="K16" s="5" t="s">
+      <c r="L16" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="1:14" ht="60" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>43355</v>
       </c>
@@ -1868,11 +1884,11 @@
       <c r="J17" s="5">
         <v>24.2</v>
       </c>
-      <c r="K17" s="8" t="s">
+      <c r="L17" s="8" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>43356</v>
       </c>
@@ -1894,11 +1910,11 @@
       <c r="J18" s="5">
         <v>24.8</v>
       </c>
-      <c r="K18" s="8" t="s">
+      <c r="L18" s="8" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>43357</v>
       </c>
@@ -1921,14 +1937,14 @@
       <c r="J19" s="5">
         <v>25.2</v>
       </c>
-      <c r="K19" s="8" t="s">
+      <c r="L19" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="L19" s="5" t="s">
+      <c r="M19" s="5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>43357</v>
       </c>
@@ -1950,14 +1966,14 @@
       <c r="J20" s="5">
         <v>30.1</v>
       </c>
-      <c r="K20" s="8" t="s">
+      <c r="L20" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="L20" s="5" t="s">
+      <c r="M20" s="5" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>43358</v>
       </c>
@@ -1977,14 +1993,14 @@
       <c r="J21" s="5">
         <v>28.1</v>
       </c>
-      <c r="K21" s="8" t="s">
+      <c r="L21" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="L21" s="5" t="s">
+      <c r="M21" s="5" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="22" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>43360</v>
       </c>
@@ -2004,14 +2020,14 @@
       <c r="J22" s="5">
         <v>31</v>
       </c>
-      <c r="K22" s="8" t="s">
+      <c r="L22" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="L22" s="5" t="s">
+      <c r="M22" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="23" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>43383</v>
       </c>
@@ -2036,17 +2052,17 @@
       <c r="J23" s="5">
         <v>28.4</v>
       </c>
-      <c r="K23" s="8" t="s">
+      <c r="L23" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="L23" s="5" t="s">
+      <c r="M23" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="N23" s="5" t="s">
+      <c r="O23" s="5" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:14" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>43384</v>
       </c>
@@ -2071,14 +2087,14 @@
       <c r="J24" s="5">
         <v>26.9</v>
       </c>
-      <c r="K24" s="8" t="s">
+      <c r="L24" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="N24" s="5" t="s">
+      <c r="O24" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="25" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>43384</v>
       </c>
@@ -2100,11 +2116,11 @@
       <c r="J25" s="5">
         <v>4.5999999999999996</v>
       </c>
-      <c r="K25" s="8" t="s">
+      <c r="L25" s="8" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>43385</v>
       </c>
@@ -2127,23 +2143,23 @@
       <c r="J26" s="5">
         <v>17.3</v>
       </c>
-      <c r="K26" s="8" t="s">
+      <c r="L26" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="E27" s="6" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="E28" s="6" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>43385</v>
       </c>
@@ -2165,32 +2181,32 @@
       <c r="J29" s="5">
         <v>28.6</v>
       </c>
-      <c r="K29" s="8" t="s">
+      <c r="L29" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="N29" s="5" t="s">
+      <c r="O29" s="5" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="E30" s="6" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="E31" s="6" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="E32" s="6" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>43385</v>
       </c>
@@ -2213,14 +2229,15 @@
       <c r="J33" s="9">
         <v>32.700000000000003</v>
       </c>
-      <c r="K33" s="5" t="s">
+      <c r="K33" s="9"/>
+      <c r="L33" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="N33" s="5" t="s">
+      <c r="O33" s="5" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" s="7">
         <v>43386</v>
       </c>
@@ -2243,14 +2260,14 @@
       <c r="J34" s="5">
         <v>30.6</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="L34" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="N34" s="5" t="s">
+      <c r="O34" s="5" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>43387</v>
       </c>
@@ -2273,14 +2290,14 @@
       <c r="J35" s="5">
         <v>22</v>
       </c>
-      <c r="K35" s="5" t="s">
+      <c r="L35" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="N35" s="5" t="s">
+      <c r="O35" s="5" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>43388</v>
       </c>
@@ -2303,14 +2320,14 @@
       <c r="J36" s="5">
         <v>6.1</v>
       </c>
-      <c r="K36" s="5" t="s">
+      <c r="L36" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="N36" s="5" t="s">
+      <c r="O36" s="5" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>43388</v>
       </c>
@@ -2333,20 +2350,20 @@
       <c r="J37" s="5">
         <v>6.7</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="L37" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="N37" s="5" t="s">
+      <c r="O37" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="E38" s="6" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" s="7">
         <v>43389</v>
       </c>
@@ -2369,14 +2386,14 @@
       <c r="J39" s="5">
         <v>30.6</v>
       </c>
-      <c r="K39" s="5" t="s">
+      <c r="L39" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="N39" s="5" t="s">
+      <c r="O39" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="1:14" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="7">
         <v>43389</v>
       </c>
@@ -2398,14 +2415,14 @@
       <c r="J40" s="5">
         <v>27.9</v>
       </c>
-      <c r="K40" s="8" t="s">
+      <c r="L40" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="N40" s="5" t="s">
+      <c r="O40" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="7">
         <v>43389</v>
       </c>
@@ -2427,11 +2444,11 @@
       <c r="J41" s="5">
         <v>28.2</v>
       </c>
-      <c r="K41" s="8" t="s">
+      <c r="L41" s="8" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>43390</v>
       </c>
@@ -2453,11 +2470,11 @@
       <c r="J42" s="5">
         <v>30.9</v>
       </c>
-      <c r="K42" s="5" t="s">
+      <c r="L42" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" s="7">
         <v>43391</v>
       </c>
@@ -2476,11 +2493,11 @@
       <c r="J43" s="5">
         <v>27.1</v>
       </c>
-      <c r="K43" s="5" t="s">
+      <c r="L43" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" s="7">
         <v>43391</v>
       </c>
@@ -2502,11 +2519,12 @@
       <c r="J44" s="9">
         <v>33.6</v>
       </c>
-      <c r="L44" s="5" t="s">
+      <c r="K44" s="9"/>
+      <c r="M44" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="E45" s="6" t="s">
         <v>112</v>
@@ -2523,11 +2541,11 @@
       <c r="J45" s="5">
         <v>32.5</v>
       </c>
-      <c r="K45" s="5" t="s">
+      <c r="L45" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="E46" s="6" t="s">
         <v>112</v>
@@ -2544,11 +2562,11 @@
       <c r="J46" s="5">
         <v>32.700000000000003</v>
       </c>
-      <c r="K46" s="5" t="s">
+      <c r="L46" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="E47" s="6" t="s">
         <v>113</v>
@@ -2565,11 +2583,11 @@
       <c r="J47" s="5">
         <v>33.200000000000003</v>
       </c>
-      <c r="K47" s="5" t="s">
+      <c r="L47" s="5" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="120" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:15" ht="120" x14ac:dyDescent="0.25">
       <c r="A48" s="7">
         <v>43392</v>
       </c>
@@ -2591,14 +2609,15 @@
       <c r="J48" s="9">
         <v>62</v>
       </c>
-      <c r="K48" s="8" t="s">
+      <c r="K48" s="9"/>
+      <c r="L48" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="L48" s="5" t="s">
+      <c r="M48" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>43397</v>
       </c>
@@ -2617,9 +2636,10 @@
       <c r="J49" s="10">
         <v>58.6</v>
       </c>
-      <c r="K49" s="8"/>
-    </row>
-    <row r="50" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K49" s="10"/>
+      <c r="L49" s="8"/>
+    </row>
+    <row r="50" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A50" s="7">
         <v>43397</v>
       </c>
@@ -2636,11 +2656,12 @@
         <v>50</v>
       </c>
       <c r="J50" s="9"/>
-      <c r="K50" s="8" t="s">
+      <c r="K50" s="9"/>
+      <c r="L50" s="8" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="7">
         <v>43398</v>
       </c>
@@ -2659,11 +2680,12 @@
       <c r="J51" s="9">
         <v>65.3</v>
       </c>
-      <c r="K51" s="5" t="s">
+      <c r="K51" s="9"/>
+      <c r="L51" s="5" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>43398</v>
       </c>
@@ -2685,11 +2707,12 @@
       <c r="J52" s="10">
         <v>62.7</v>
       </c>
-      <c r="K52" s="5" t="s">
+      <c r="K52" s="10"/>
+      <c r="L52" s="5" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="7">
         <v>43398</v>
       </c>
@@ -2702,11 +2725,12 @@
       <c r="J53" s="9">
         <v>63.6</v>
       </c>
-      <c r="K53" s="5" t="s">
+      <c r="K53" s="9"/>
+      <c r="L53" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="7">
         <v>43398</v>
       </c>
@@ -2728,11 +2752,12 @@
       <c r="J54" s="9">
         <v>63.4</v>
       </c>
-      <c r="K54" s="5" t="s">
+      <c r="K54" s="9"/>
+      <c r="L54" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="55" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>43399</v>
       </c>
@@ -2740,7 +2765,7 @@
         <v>44</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G55" s="5">
         <v>24</v>
@@ -2754,8 +2779,9 @@
       <c r="J55" s="11">
         <v>56.7</v>
       </c>
-    </row>
-    <row r="56" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K55" s="11"/>
+    </row>
+    <row r="56" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A56" s="7">
         <v>43399</v>
       </c>
@@ -2765,11 +2791,11 @@
       <c r="J56" s="5">
         <v>54.6</v>
       </c>
-      <c r="K56" s="8" t="s">
+      <c r="L56" s="8" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="57" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="7">
         <v>43399</v>
       </c>
@@ -2788,11 +2814,12 @@
       <c r="J57" s="9">
         <v>65.099999999999994</v>
       </c>
-      <c r="K57" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K57" s="9"/>
+      <c r="L57" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="58" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="7">
         <v>43418</v>
       </c>
@@ -2800,7 +2827,7 @@
         <v>46</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H58" s="5">
         <v>113</v>
@@ -2811,11 +2838,11 @@
       <c r="J58" s="5">
         <v>43.8</v>
       </c>
-      <c r="K58" s="5" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="59" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L58" s="5" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="7">
         <v>43419</v>
       </c>
@@ -2823,7 +2850,7 @@
         <v>47</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H59" s="5">
         <v>20</v>
@@ -2834,11 +2861,11 @@
       <c r="J59" s="5">
         <v>2</v>
       </c>
-      <c r="K59" s="5" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="60" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L59" s="5" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="60" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="7">
         <v>43425</v>
       </c>
@@ -2846,7 +2873,7 @@
         <v>48</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H60" s="5">
         <v>105</v>
@@ -2857,11 +2884,12 @@
       <c r="J60" s="9">
         <v>59.3</v>
       </c>
-      <c r="K60" s="5" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="K60" s="9"/>
+      <c r="L60" s="5" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="61" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="7">
         <v>43426</v>
       </c>
@@ -2869,7 +2897,7 @@
         <v>49</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I61" s="9">
         <v>99.3</v>
@@ -2877,11 +2905,12 @@
       <c r="J61" s="12">
         <v>44.9</v>
       </c>
-      <c r="K61" s="5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="K61" s="12"/>
+      <c r="L61" s="5" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="62" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A62" s="7">
         <v>43429</v>
       </c>
@@ -2889,7 +2918,7 @@
         <v>50</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H62" s="5">
         <v>20</v>
@@ -2900,11 +2929,12 @@
       <c r="J62" s="12">
         <v>39.299999999999997</v>
       </c>
-      <c r="K62" s="8" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K62" s="12"/>
+      <c r="L62" s="8" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="7">
         <v>43430</v>
       </c>
@@ -2912,7 +2942,7 @@
         <v>51</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="H63" s="5">
         <v>142</v>
@@ -2923,11 +2953,12 @@
       <c r="J63" s="12">
         <v>55.5</v>
       </c>
-      <c r="K63" s="5" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K63" s="12"/>
+      <c r="L63" s="5" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="7">
         <v>43431</v>
       </c>
@@ -2935,7 +2966,7 @@
         <v>52</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H64" s="5">
         <v>112</v>
@@ -2946,16 +2977,17 @@
       <c r="J64" s="12">
         <v>55.6</v>
       </c>
-      <c r="K64" s="5" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K64" s="12"/>
+      <c r="L64" s="5" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="7">
         <v>43433</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H65" s="5">
         <v>118</v>
@@ -2966,16 +2998,17 @@
       <c r="J65" s="12">
         <v>58</v>
       </c>
-      <c r="K65" s="5" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K65" s="12"/>
+      <c r="L65" s="5" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="7">
         <v>43434</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H66" s="5">
         <v>95</v>
@@ -2986,16 +3019,17 @@
       <c r="J66" s="15">
         <v>58.3</v>
       </c>
-      <c r="K66" s="5" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K66" s="15"/>
+      <c r="L66" s="5" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="7">
         <v>43434</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="H67" s="5">
         <v>121</v>
@@ -3006,16 +3040,17 @@
       <c r="J67" s="9">
         <v>60.9</v>
       </c>
-      <c r="K67" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K67" s="9"/>
+      <c r="L67" s="5" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="7">
         <v>43434</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H68" s="5">
         <v>97</v>
@@ -3026,13 +3061,14 @@
       <c r="J68" s="16">
         <v>59.8</v>
       </c>
-      <c r="K68" s="5" t="s">
+      <c r="K68" s="16"/>
+      <c r="L68" s="5" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="69" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="E69" s="6" t="s">
         <v>160</v>
-      </c>
-    </row>
-    <row r="69" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="E69" s="6" t="s">
-        <v>161</v>
       </c>
       <c r="H69" s="5">
         <v>109</v>
@@ -3043,11 +3079,11 @@
       <c r="J69" s="5">
         <v>60.6</v>
       </c>
-      <c r="K69" s="5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="70" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="L69" s="5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A70" s="7">
         <v>43437</v>
       </c>
@@ -3055,7 +3091,7 @@
         <v>53</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="H70" s="5">
         <v>125</v>
@@ -3066,13 +3102,16 @@
       <c r="J70" s="5">
         <v>60.4</v>
       </c>
-      <c r="K70" s="5" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L70" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="7">
+        <v>43438</v>
+      </c>
       <c r="E71" s="6" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H71" s="5">
         <v>165</v>
@@ -3083,13 +3122,16 @@
       <c r="J71" s="9">
         <v>61.2</v>
       </c>
-      <c r="K71" s="5" t="s">
+      <c r="K71" s="5">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A72" s="7">
+        <v>43438</v>
+      </c>
+      <c r="E72" s="6" t="s">
         <v>165</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="E72" s="6" t="s">
-        <v>168</v>
       </c>
       <c r="H72" s="5">
         <v>205</v>
@@ -3100,13 +3142,16 @@
       <c r="J72" s="9">
         <v>61.4</v>
       </c>
-      <c r="K72" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="K72" s="5">
+        <v>87.2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A73" s="7">
+        <v>43438</v>
+      </c>
       <c r="E73" s="6" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="H73" s="5">
         <v>260</v>
@@ -3117,13 +3162,16 @@
       <c r="J73" s="9">
         <v>61.7</v>
       </c>
-      <c r="K73" s="5" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="74" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="K73" s="5">
+        <v>87.9</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A74" s="7">
+        <v>43438</v>
+      </c>
       <c r="E74" s="6" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="H74" s="5">
         <v>311</v>
@@ -3134,13 +3182,16 @@
       <c r="J74" s="9">
         <v>62</v>
       </c>
-      <c r="K74" s="5" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K74" s="5">
+        <v>87.2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="7">
+        <v>43438</v>
+      </c>
       <c r="E75" s="6" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="H75" s="5">
         <v>194</v>
@@ -3151,46 +3202,112 @@
       <c r="J75" s="17">
         <v>57.9</v>
       </c>
-      <c r="K75" s="5" t="s">
+      <c r="K75" s="5">
+        <v>84.4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="7">
+        <v>43439</v>
+      </c>
+      <c r="E76" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="H76" s="5">
+        <v>136</v>
+      </c>
+      <c r="I76" s="5">
+        <v>89.7</v>
+      </c>
+      <c r="J76" s="17">
+        <v>60.9</v>
+      </c>
+      <c r="K76" s="5">
+        <v>86.8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" s="7">
+        <v>43439</v>
+      </c>
+      <c r="E77" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="H77" s="5">
+        <v>161</v>
+      </c>
+      <c r="I77" s="5">
+        <v>96.8</v>
+      </c>
+      <c r="J77" s="9">
+        <v>62.5</v>
+      </c>
+      <c r="K77" s="17">
+        <v>87.3</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" s="7">
+        <v>43439</v>
+      </c>
+      <c r="E78" s="6" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E76" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="J76" s="17"/>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="J77" s="9"/>
-    </row>
-    <row r="78" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="E78" s="6" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H78" s="5">
+        <v>138</v>
+      </c>
+      <c r="I78" s="5">
+        <v>93.4</v>
+      </c>
+      <c r="J78" s="18">
+        <v>61.4</v>
+      </c>
+      <c r="K78" s="18">
+        <v>86.9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" s="7">
+        <v>43441</v>
+      </c>
       <c r="E79" s="6" t="s">
+        <v>173</v>
+      </c>
+      <c r="H79" s="5">
+        <v>119</v>
+      </c>
+      <c r="I79" s="5">
+        <v>88</v>
+      </c>
+      <c r="J79" s="9">
+        <v>59.9</v>
+      </c>
+      <c r="K79" s="9">
+        <v>83.9</v>
+      </c>
+    </row>
+    <row r="83" spans="5:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="E83" s="6" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E84" s="6" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="E80" s="6" t="s">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E85" s="6" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E81" s="6" t="s">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E86" s="6" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E82" s="6" t="s">
-        <v>135</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:L19">
+  <autoFilter ref="A1:M19">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
confidence and accuracy dependency
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="196">
   <si>
     <t>No</t>
   </si>
@@ -967,6 +967,12 @@
   </si>
   <si>
     <t>Pretrained vgg minus last layer (1000 cl) + last layer (100)</t>
+  </si>
+  <si>
+    <t>Pretrained vgg + last layer (100)</t>
+  </si>
+  <si>
+    <t>Better</t>
   </si>
 </sst>
 </file>
@@ -1503,8 +1509,8 @@
   <dimension ref="A1:O105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A81" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A91" activeCellId="1" sqref="A82:XFD82 A91:XFD91"/>
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L92" sqref="L92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3628,15 +3634,12 @@
         <v>190</v>
       </c>
     </row>
-    <row r="91" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="9">
         <v>43452</v>
       </c>
-      <c r="C91" s="7">
-        <v>59</v>
-      </c>
       <c r="E91" s="6" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="H91" s="7">
         <v>35</v>
@@ -3654,8 +3657,31 @@
         <v>192</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A92" s="9"/>
+    <row r="92" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A92" s="9">
+        <v>43461</v>
+      </c>
+      <c r="C92" s="7">
+        <v>59</v>
+      </c>
+      <c r="E92" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="H92" s="7">
+        <v>25</v>
+      </c>
+      <c r="I92" s="7">
+        <v>87.1</v>
+      </c>
+      <c r="J92" s="10">
+        <v>77.8</v>
+      </c>
+      <c r="K92" s="10">
+        <v>94.7</v>
+      </c>
+      <c r="L92" s="7" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="102" spans="5:5" ht="30" x14ac:dyDescent="0.25">
       <c r="E102" s="6" t="s">

</xml_diff>

<commit_message>
just more det experiments
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9210"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9210" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Classification" sheetId="1" r:id="rId1"/>
+    <sheet name="Detection" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Classification!$A$1:$M$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Detection!$A$1:$H$19</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="239">
   <si>
     <t>No</t>
   </si>
@@ -260,12 +261,6 @@
       </rPr>
       <t>144 passes through data)</t>
     </r>
-  </si>
-  <si>
-    <t>batch size</t>
-  </si>
-  <si>
-    <t>train duration per 1 subframe, secs</t>
   </si>
   <si>
     <t>model_v18.h5</t>
@@ -985,6 +980,146 @@
   </si>
   <si>
     <t>Pretrained vgg (1000=&gt;100); train D2 and softmax</t>
+  </si>
+  <si>
+    <t>v63</t>
+  </si>
+  <si>
+    <t>5CNN + 3 Dense. BN before dense. Bbox sigmoid act.</t>
+  </si>
+  <si>
+    <t>Train loss</t>
+  </si>
+  <si>
+    <t>Test loss</t>
+  </si>
+  <si>
+    <t>Bbox sigmoid==&gt;linear activation</t>
+  </si>
+  <si>
+    <t>v64</t>
+  </si>
+  <si>
+    <t>v65</t>
+  </si>
+  <si>
+    <t>Change pre-process function from vgg to /255</t>
+  </si>
+  <si>
+    <t>Not better; mosty all images have predicted bbox in central frame (2,2 from 3x3) with high probability</t>
+  </si>
+  <si>
+    <t>Subdivisions 3==&gt;19</t>
+  </si>
+  <si>
+    <t>All pr_obj=0.0; all bboxes high numbers (mean ~150.). Looks like significance of bbox needs to be reduced in respect to Pr(Obj)</t>
+  </si>
+  <si>
+    <t>v66</t>
+  </si>
+  <si>
+    <t>v67</t>
+  </si>
+  <si>
+    <t>Bbox loss mse=&gt;sqrt(mse)</t>
+  </si>
+  <si>
+    <t>Reduce significance of bbox error even more sqrt(mse) =&gt; sqrt(mse)/4</t>
+  </si>
+  <si>
+    <t>Loss not comparable to above tests. Most Pr_obj&lt;0.25.
+Sample error(pr_obj)=0.01. Sample error(bbox)=0.08</t>
+  </si>
+  <si>
+    <t>v68</t>
+  </si>
+  <si>
+    <t>Sample error(pr_obj)=0.009. Sample error(bbox)=0.013. Similar, good
+Bboxes still nonsense. Most Pr_obj&lt;0.25 - penalize differently Pr(obj) and Pr(noobj)</t>
+  </si>
+  <si>
+    <t>Add bigger penalty for FN than for FP (because most subdivisions don't contain objects, pr_obj tends to be reduced to close to 0). According to Yolo paper, coef= 0.5
+(also, taking sum or Pr_obj error rather that mean. This reduces the significance of error(bbox), but will later work on it</t>
+  </si>
+  <si>
+    <t>Sample error distribution:
+Loss_pr_obj: 102.76862
+Loss_pr_noobj: 2.6558914
+Loss_bbox: 0.022595681
+Need to increase penalty for pr_obj</t>
+  </si>
+  <si>
+    <t>Change lambda_noobj 0.5=&gt;0.05</t>
+  </si>
+  <si>
+    <t>Add momentum of 0.0==&gt;0.9</t>
+  </si>
+  <si>
+    <t>Did not converge. Maybe add momentum?
+Sample error distribution:
+Loss_pr_obj: 91.086685  (down a bit); Loss_pr_noobj: 391.2927; Loss_bbox: 0.021647379
+Mean pr_obj = 0.04. Quite reasonable</t>
+  </si>
+  <si>
+    <t>Huge activations before BN layer (in CNN)
+Loss_pr_obj: 90.99968; Loss_pr_noobj: 229.02045; Loss_bbox: 0.02045007
+Momentum didn't help
+most samples contain 2 pr_obj=1. All pr_obj on extreme end (0 or 1)</t>
+  </si>
+  <si>
+    <t>Ideas</t>
+  </si>
+  <si>
+    <t>Add BN in between CNN layers</t>
+  </si>
+  <si>
+    <t>Add BN after 2nd CNN layer (before mean was 192, std 400)</t>
+  </si>
+  <si>
+    <t>v69</t>
+  </si>
+  <si>
+    <t>Mean/std of 4th cnn is 20/40. Still very big activations of last cnn</t>
+  </si>
+  <si>
+    <t>Add BN in after 4th CNN layers</t>
+  </si>
+  <si>
+    <t>Add BN after 4th layer</t>
+  </si>
+  <si>
+    <t>Loss_pr_obj: 95.0; Loss_pr_noobj: 242.0; Loss_bbox: 0.086606294; Loss: 107.12165
+pr_obj still extreme :(
+dense_1 activation mean/std 82/666</t>
+  </si>
+  <si>
+    <t>Instead of BN after dense_1, change to BN after flatten</t>
+  </si>
+  <si>
+    <t>BN from (after dense1) to (before dense1)</t>
+  </si>
+  <si>
+    <t>6X</t>
+  </si>
+  <si>
+    <t>1XX</t>
+  </si>
+  <si>
+    <t>All pr_obj==&gt;0</t>
+  </si>
+  <si>
+    <t>Loss likely went up due to higher bbox error variance (sigmoid=&gt;linear)
+Huge learnt variance values of batch normalization layer (used BN w/o beta, gama)</t>
+  </si>
+  <si>
+    <t>v71</t>
+  </si>
+  <si>
+    <t>3cnn, 2 dense</t>
+  </si>
+  <si>
+    <t>Loss_pr_obj: 48.999825; Loss_pr_noobj: 177.0; Loss_bbox: 0.016190218
+cnn activations=0</t>
   </si>
 </sst>
 </file>
@@ -1147,7 +1282,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -1203,6 +1338,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1520,7 +1656,7 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:O105"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L95" sqref="L95"/>
     </sheetView>
@@ -1561,7 +1697,7 @@
         <v>7</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>6</v>
@@ -1573,7 +1709,7 @@
         <v>4</v>
       </c>
       <c r="K1" s="8" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L1" s="8" t="s">
         <v>5</v>
@@ -2135,7 +2271,7 @@
         <v>53</v>
       </c>
       <c r="M22" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="90" x14ac:dyDescent="0.25">
@@ -2143,13 +2279,13 @@
         <v>43383</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C23" s="7">
         <v>19</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G23" s="5">
         <v>10</v>
@@ -2164,13 +2300,13 @@
         <v>28.4</v>
       </c>
       <c r="L23" s="7" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O23" s="7" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="45" x14ac:dyDescent="0.25">
@@ -2178,13 +2314,13 @@
         <v>43384</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C24" s="7">
         <v>20</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G24" s="5">
         <v>5</v>
@@ -2199,10 +2335,10 @@
         <v>26.9</v>
       </c>
       <c r="L24" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="O24" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -2213,7 +2349,7 @@
         <v>21</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G25" s="5">
         <v>1</v>
@@ -2228,7 +2364,7 @@
         <v>4.5999999999999996</v>
       </c>
       <c r="L25" s="7" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.25">
@@ -2239,7 +2375,7 @@
         <v>23</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="G26" s="5">
         <v>3</v>
@@ -2255,19 +2391,19 @@
         <v>17.3</v>
       </c>
       <c r="L26" s="7" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="9"/>
       <c r="E27" s="6" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" s="9"/>
       <c r="E28" s="6" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.25">
@@ -2278,7 +2414,7 @@
         <v>26</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G29" s="5">
         <v>2</v>
@@ -2293,28 +2429,28 @@
         <v>28.6</v>
       </c>
       <c r="L29" s="7" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="O29" s="7" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" s="9"/>
       <c r="E30" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" s="9"/>
       <c r="E31" s="6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" s="9"/>
       <c r="E32" s="6" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
@@ -2325,7 +2461,7 @@
         <v>30</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G33" s="5">
         <v>3</v>
@@ -2342,10 +2478,10 @@
       </c>
       <c r="K33" s="10"/>
       <c r="L33" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="O33" s="7" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
@@ -2356,7 +2492,7 @@
         <v>31</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G34" s="5">
         <v>3</v>
@@ -2372,10 +2508,10 @@
         <v>30.6</v>
       </c>
       <c r="L34" s="7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="O34" s="7" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="35" spans="1:15" x14ac:dyDescent="0.25">
@@ -2386,7 +2522,7 @@
         <v>32</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G35" s="5">
         <v>3</v>
@@ -2402,10 +2538,10 @@
         <v>22</v>
       </c>
       <c r="L35" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="O35" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.25">
@@ -2416,7 +2552,7 @@
         <v>33</v>
       </c>
       <c r="E36" s="6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G36" s="5">
         <v>3</v>
@@ -2432,10 +2568,10 @@
         <v>6.1</v>
       </c>
       <c r="L36" s="7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="O36" s="7" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.25">
@@ -2446,7 +2582,7 @@
         <v>34</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G37" s="5">
         <v>3</v>
@@ -2462,16 +2598,16 @@
         <v>6.7</v>
       </c>
       <c r="L37" s="7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="O37" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" s="9"/>
       <c r="E38" s="6" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="39" spans="1:15" x14ac:dyDescent="0.25">
@@ -2482,7 +2618,7 @@
         <v>35</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G39" s="5">
         <v>3</v>
@@ -2498,10 +2634,10 @@
         <v>30.6</v>
       </c>
       <c r="L39" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="O39" s="7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2512,7 +2648,7 @@
         <v>36</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G40" s="5">
         <v>1</v>
@@ -2527,10 +2663,10 @@
         <v>27.9</v>
       </c>
       <c r="L40" s="7" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="O40" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -2541,7 +2677,7 @@
         <v>37</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G41" s="5">
         <v>1</v>
@@ -2556,7 +2692,7 @@
         <v>28.2</v>
       </c>
       <c r="L41" s="7" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.25">
@@ -2567,7 +2703,7 @@
         <v>38</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G42" s="5">
         <v>1</v>
@@ -2582,7 +2718,7 @@
         <v>30.9</v>
       </c>
       <c r="L42" s="7" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.25">
@@ -2590,7 +2726,7 @@
         <v>43391</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G43" s="5">
         <v>10</v>
@@ -2605,7 +2741,7 @@
         <v>27.1</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="30" x14ac:dyDescent="0.25">
@@ -2616,7 +2752,7 @@
         <v>39</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G44" s="5">
         <v>50</v>
@@ -2632,13 +2768,13 @@
       </c>
       <c r="K44" s="10"/>
       <c r="M44" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" s="9"/>
       <c r="E45" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G45" s="5">
         <v>100</v>
@@ -2653,13 +2789,13 @@
         <v>32.5</v>
       </c>
       <c r="L45" s="7" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" s="9"/>
       <c r="E46" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G46" s="5">
         <v>150</v>
@@ -2674,13 +2810,13 @@
         <v>32.700000000000003</v>
       </c>
       <c r="L46" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" s="9"/>
       <c r="E47" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="G47" s="5">
         <v>100</v>
@@ -2695,7 +2831,7 @@
         <v>33.200000000000003</v>
       </c>
       <c r="L47" s="7" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="120" x14ac:dyDescent="0.25">
@@ -2706,7 +2842,7 @@
         <v>40</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G48" s="5">
         <v>50</v>
@@ -2722,10 +2858,10 @@
       </c>
       <c r="K48" s="10"/>
       <c r="L48" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="M48" s="7" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
@@ -2733,7 +2869,7 @@
         <v>43397</v>
       </c>
       <c r="E49" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G49" s="5">
         <v>50</v>
@@ -2757,7 +2893,7 @@
         <v>41</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G50" s="5">
         <v>50</v>
@@ -2768,7 +2904,7 @@
       <c r="J50" s="10"/>
       <c r="K50" s="10"/>
       <c r="L50" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -2776,7 +2912,7 @@
         <v>43398</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G51" s="5">
         <v>50</v>
@@ -2792,7 +2928,7 @@
       </c>
       <c r="K51" s="10"/>
       <c r="L51" s="7" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -2803,7 +2939,7 @@
         <v>42</v>
       </c>
       <c r="E52" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="G52" s="5">
         <v>50</v>
@@ -2819,7 +2955,7 @@
       </c>
       <c r="K52" s="11"/>
       <c r="L52" s="7" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -2827,7 +2963,7 @@
         <v>43398</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="I53" s="7">
         <v>80.8</v>
@@ -2837,7 +2973,7 @@
       </c>
       <c r="K53" s="10"/>
       <c r="L53" s="7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -2848,7 +2984,7 @@
         <v>43</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G54" s="5">
         <v>100</v>
@@ -2864,7 +3000,7 @@
       </c>
       <c r="K54" s="10"/>
       <c r="L54" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="55" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2875,7 +3011,7 @@
         <v>44</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="G55" s="5">
         <v>24</v>
@@ -2896,13 +3032,13 @@
         <v>43399</v>
       </c>
       <c r="E56" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="J56" s="7">
         <v>54.6</v>
       </c>
       <c r="L56" s="7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="57" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2913,7 +3049,7 @@
         <v>45</v>
       </c>
       <c r="E57" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H57" s="7">
         <v>83</v>
@@ -2926,7 +3062,7 @@
       </c>
       <c r="K57" s="10"/>
       <c r="L57" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2937,7 +3073,7 @@
         <v>46</v>
       </c>
       <c r="E58" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H58" s="7">
         <v>113</v>
@@ -2949,7 +3085,7 @@
         <v>43.8</v>
       </c>
       <c r="L58" s="7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2960,7 +3096,7 @@
         <v>47</v>
       </c>
       <c r="E59" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H59" s="7">
         <v>20</v>
@@ -2972,7 +3108,7 @@
         <v>2</v>
       </c>
       <c r="L59" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="60" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -2983,7 +3119,7 @@
         <v>48</v>
       </c>
       <c r="E60" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H60" s="7">
         <v>105</v>
@@ -2996,7 +3132,7 @@
       </c>
       <c r="K60" s="10"/>
       <c r="L60" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="61" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3007,7 +3143,7 @@
         <v>49</v>
       </c>
       <c r="E61" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="I61" s="10">
         <v>99.3</v>
@@ -3017,7 +3153,7 @@
       </c>
       <c r="K61" s="13"/>
       <c r="L61" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="62" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -3028,7 +3164,7 @@
         <v>50</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H62" s="7">
         <v>20</v>
@@ -3041,7 +3177,7 @@
       </c>
       <c r="K62" s="13"/>
       <c r="L62" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="63" spans="1:12" x14ac:dyDescent="0.25">
@@ -3052,7 +3188,7 @@
         <v>51</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H63" s="7">
         <v>142</v>
@@ -3065,7 +3201,7 @@
       </c>
       <c r="K63" s="13"/>
       <c r="L63" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="64" spans="1:12" x14ac:dyDescent="0.25">
@@ -3076,7 +3212,7 @@
         <v>52</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H64" s="7">
         <v>112</v>
@@ -3089,7 +3225,7 @@
       </c>
       <c r="K64" s="13"/>
       <c r="L64" s="7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="65" spans="1:12" x14ac:dyDescent="0.25">
@@ -3097,7 +3233,7 @@
         <v>43433</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="H65" s="7">
         <v>118</v>
@@ -3110,7 +3246,7 @@
       </c>
       <c r="K65" s="13"/>
       <c r="L65" s="7" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.25">
@@ -3118,7 +3254,7 @@
         <v>43434</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="H66" s="7">
         <v>95</v>
@@ -3131,7 +3267,7 @@
       </c>
       <c r="K66" s="16"/>
       <c r="L66" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -3139,7 +3275,7 @@
         <v>43434</v>
       </c>
       <c r="E67" s="6" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="H67" s="7">
         <v>121</v>
@@ -3152,7 +3288,7 @@
       </c>
       <c r="K67" s="10"/>
       <c r="L67" s="7" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.25">
@@ -3160,7 +3296,7 @@
         <v>43434</v>
       </c>
       <c r="E68" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="H68" s="7">
         <v>97</v>
@@ -3173,12 +3309,12 @@
       </c>
       <c r="K68" s="17"/>
       <c r="L68" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="69" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="E69" s="6" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="H69" s="7">
         <v>109</v>
@@ -3193,7 +3329,7 @@
         <v>87.5</v>
       </c>
       <c r="L69" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="70" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3204,7 +3340,7 @@
         <v>53</v>
       </c>
       <c r="E70" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="H70" s="7">
         <v>125</v>
@@ -3219,7 +3355,7 @@
         <v>87.1</v>
       </c>
       <c r="L70" s="7" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
@@ -3227,7 +3363,7 @@
         <v>43438</v>
       </c>
       <c r="E71" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="H71" s="7">
         <v>165</v>
@@ -3247,7 +3383,7 @@
         <v>43438</v>
       </c>
       <c r="E72" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="H72" s="7">
         <v>205</v>
@@ -3267,7 +3403,7 @@
         <v>43438</v>
       </c>
       <c r="E73" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="H73" s="7">
         <v>260</v>
@@ -3287,7 +3423,7 @@
         <v>43438</v>
       </c>
       <c r="E74" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H74" s="7">
         <v>311</v>
@@ -3307,7 +3443,7 @@
         <v>43438</v>
       </c>
       <c r="E75" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H75" s="7">
         <v>194</v>
@@ -3327,7 +3463,7 @@
         <v>43439</v>
       </c>
       <c r="E76" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="H76" s="7">
         <v>136</v>
@@ -3347,7 +3483,7 @@
         <v>43439</v>
       </c>
       <c r="E77" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H77" s="7">
         <v>161</v>
@@ -3367,7 +3503,7 @@
         <v>43439</v>
       </c>
       <c r="E78" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H78" s="7">
         <v>138</v>
@@ -3390,7 +3526,7 @@
         <v>54</v>
       </c>
       <c r="E79" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H79" s="7">
         <v>119</v>
@@ -3405,7 +3541,7 @@
         <v>83.9</v>
       </c>
       <c r="L79" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="80" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3413,7 +3549,7 @@
         <v>43441</v>
       </c>
       <c r="E80" s="6" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H80" s="7">
         <v>150</v>
@@ -3433,7 +3569,7 @@
         <v>43441</v>
       </c>
       <c r="E81" s="6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H81" s="7">
         <v>179</v>
@@ -3453,7 +3589,7 @@
         <v>43441</v>
       </c>
       <c r="E82" s="6" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H82" s="7">
         <v>204</v>
@@ -3473,7 +3609,7 @@
         <v>43441</v>
       </c>
       <c r="E83" s="6" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H83" s="7">
         <v>259</v>
@@ -3493,7 +3629,7 @@
         <v>43441</v>
       </c>
       <c r="E84" s="6" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H84" s="7">
         <v>280</v>
@@ -3516,7 +3652,7 @@
         <v>55</v>
       </c>
       <c r="E85" s="6" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H85" s="7">
         <v>98</v>
@@ -3531,7 +3667,7 @@
         <v>84.6</v>
       </c>
       <c r="L85" s="7" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="86" spans="1:12" x14ac:dyDescent="0.25">
@@ -3542,7 +3678,7 @@
         <v>56</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H86" s="7">
         <v>135</v>
@@ -3559,7 +3695,7 @@
     </row>
     <row r="87" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="E87" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H87" s="7">
         <v>103</v>
@@ -3574,7 +3710,7 @@
         <v>84.8</v>
       </c>
       <c r="L87" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="88" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3585,10 +3721,10 @@
         <v>57</v>
       </c>
       <c r="E88" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="H88" s="7" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J88" s="10">
         <v>68.5</v>
@@ -3597,7 +3733,7 @@
         <v>88.3</v>
       </c>
       <c r="L88" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="89" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -3608,7 +3744,7 @@
         <v>58</v>
       </c>
       <c r="E89" s="6" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="H89" s="7">
         <v>20</v>
@@ -3620,7 +3756,7 @@
         <v>99</v>
       </c>
       <c r="L89" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="90" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3628,7 +3764,7 @@
         <v>43451</v>
       </c>
       <c r="E90" s="6" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="H90" s="7">
         <v>82</v>
@@ -3643,7 +3779,7 @@
         <v>83.3</v>
       </c>
       <c r="L90" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.25">
@@ -3651,7 +3787,7 @@
         <v>43452</v>
       </c>
       <c r="E91" s="6" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="H91" s="7">
         <v>35</v>
@@ -3666,7 +3802,7 @@
         <v>93.5</v>
       </c>
       <c r="L91" s="7" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="92" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -3677,7 +3813,7 @@
         <v>59</v>
       </c>
       <c r="E92" s="6" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="H92" s="7">
         <v>25</v>
@@ -3692,7 +3828,7 @@
         <v>94.7</v>
       </c>
       <c r="L92" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.25">
@@ -3700,7 +3836,7 @@
         <v>43462</v>
       </c>
       <c r="E93" s="6" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="H93" s="7">
         <v>22</v>
@@ -3715,7 +3851,7 @@
         <v>94.9</v>
       </c>
       <c r="L93" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.25">
@@ -3723,7 +3859,7 @@
         <v>43464</v>
       </c>
       <c r="E94" s="6" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="H94" s="7">
         <v>50</v>
@@ -3746,7 +3882,7 @@
         <v>60</v>
       </c>
       <c r="E95" s="6" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="H95" s="7">
         <v>25</v>
@@ -3763,22 +3899,22 @@
     </row>
     <row r="102" spans="5:5" ht="30" x14ac:dyDescent="0.25">
       <c r="E102" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="103" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E103" s="6" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="104" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E104" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="105" spans="5:5" x14ac:dyDescent="0.25">
       <c r="E105" s="6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -3794,59 +3930,664 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:I95"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="49" customWidth="1"/>
+    <col min="1" max="1" width="7.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="5.140625" style="7" customWidth="1"/>
+    <col min="4" max="4" width="50.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="11.140625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="87.140625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="22.28515625" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>32</v>
-      </c>
-      <c r="B2">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>64</v>
-      </c>
-      <c r="B3">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>128</v>
-      </c>
-      <c r="B4">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>256</v>
-      </c>
-      <c r="B5">
-        <v>37</v>
-      </c>
+    <row r="1" spans="1:9" s="8" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>43553</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" s="7">
+        <v>1</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>199</v>
+      </c>
+      <c r="E2" s="7">
+        <v>7</v>
+      </c>
+      <c r="F2" s="7">
+        <v>0.21990000000000001</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0.33150000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" s="5" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="21">
+        <v>43553</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="E3" s="5">
+        <v>7</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0.27079999999999999</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0.39150000000000001</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="5" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="21">
+        <v>43556</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="C4" s="5">
+        <v>3</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="E4" s="5">
+        <v>7</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.22239999999999999</v>
+      </c>
+      <c r="G4" s="5">
+        <v>0.51319999999999999</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>43558</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>209</v>
+      </c>
+      <c r="C5" s="7">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="E5" s="7">
+        <v>7</v>
+      </c>
+      <c r="F5" s="7">
+        <v>0.26090000000000002</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.3982</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>43559</v>
+      </c>
+      <c r="C6" s="7">
+        <v>5</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E6" s="7">
+        <v>7</v>
+      </c>
+      <c r="F6" s="7">
+        <v>8.0799999999999997E-2</v>
+      </c>
+      <c r="G6" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="21">
+        <v>43559</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="C7" s="5">
+        <v>6</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>212</v>
+      </c>
+      <c r="E7" s="5">
+        <v>5</v>
+      </c>
+      <c r="F7" s="5">
+        <v>3.27E-2</v>
+      </c>
+      <c r="G7" s="5">
+        <v>2.5100000000000001E-2</v>
+      </c>
+      <c r="H7" s="7" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" s="5" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A8" s="21">
+        <v>43559</v>
+      </c>
+      <c r="B8" s="21"/>
+      <c r="C8" s="5">
+        <v>7</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E8" s="5">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5">
+        <v>65.790000000000006</v>
+      </c>
+      <c r="G8" s="5">
+        <v>169.39</v>
+      </c>
+      <c r="H8" s="7" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>43560</v>
+      </c>
+      <c r="C9" s="7">
+        <v>8</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="E9" s="7">
+        <v>5</v>
+      </c>
+      <c r="F9" s="7">
+        <v>48</v>
+      </c>
+      <c r="G9" s="7">
+        <v>136</v>
+      </c>
+      <c r="H9" s="7" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>43560</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="7">
+        <v>9</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="E10" s="7">
+        <v>5</v>
+      </c>
+      <c r="F10" s="7">
+        <v>58.6</v>
+      </c>
+      <c r="G10" s="7">
+        <v>169</v>
+      </c>
+      <c r="H10" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="I10" s="7" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>43563</v>
+      </c>
+      <c r="B11" s="9"/>
+      <c r="D11" s="6" t="s">
+        <v>224</v>
+      </c>
+      <c r="E11" s="7">
+        <v>5</v>
+      </c>
+      <c r="F11" s="7">
+        <v>63.1</v>
+      </c>
+      <c r="G11" s="7">
+        <v>169</v>
+      </c>
+      <c r="H11" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="I11" s="7" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>43564</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="7">
+        <v>10</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="E12" s="7">
+        <v>5</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="G12" s="7" t="s">
+        <v>233</v>
+      </c>
+      <c r="H12" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="I12" s="7" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>43564</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="C13" s="7">
+        <v>11</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="E13" s="7">
+        <v>5</v>
+      </c>
+      <c r="F13" s="7">
+        <v>66</v>
+      </c>
+      <c r="G13" s="7">
+        <v>172</v>
+      </c>
+      <c r="H13" s="7" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>43567</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="C14" s="7">
+        <v>12</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>237</v>
+      </c>
+      <c r="E14" s="7">
+        <v>2</v>
+      </c>
+      <c r="F14" s="7">
+        <v>58</v>
+      </c>
+      <c r="H14" s="7" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="9"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="9"/>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9"/>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9"/>
+    </row>
+    <row r="19" spans="1:1" ht="40.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="9"/>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="9"/>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="9"/>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="9"/>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" s="9"/>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" s="9"/>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" s="9"/>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" s="9"/>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" s="9"/>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" s="9"/>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9"/>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9"/>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="9"/>
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="9"/>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" s="9"/>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" s="9"/>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" s="9"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="9"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="9"/>
+    </row>
+    <row r="40" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="9"/>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" s="9"/>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="9"/>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" s="9"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" s="9"/>
+      <c r="G44" s="10"/>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" s="9"/>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" s="9"/>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" s="9"/>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="9"/>
+      <c r="G48" s="10"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="9"/>
+      <c r="G49" s="11"/>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" s="9"/>
+      <c r="G50" s="10"/>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" s="9"/>
+      <c r="G51" s="10"/>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" s="9"/>
+      <c r="G52" s="11"/>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A53" s="9"/>
+      <c r="G53" s="10"/>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A54" s="9"/>
+      <c r="G54" s="10"/>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A55" s="9"/>
+      <c r="G55" s="12"/>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A56" s="9"/>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A57" s="9"/>
+      <c r="G57" s="10"/>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="9"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="9"/>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="9"/>
+      <c r="G60" s="10"/>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="9"/>
+      <c r="F61" s="10"/>
+      <c r="G61" s="13"/>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="9"/>
+      <c r="F62" s="14"/>
+      <c r="G62" s="13"/>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="9"/>
+      <c r="F63" s="15"/>
+      <c r="G63" s="13"/>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="9"/>
+      <c r="F64" s="15"/>
+      <c r="G64" s="13"/>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="9"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="13"/>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="9"/>
+      <c r="G66" s="16"/>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" s="9"/>
+      <c r="G67" s="10"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A68" s="9"/>
+      <c r="G68" s="17"/>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A70" s="9"/>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A71" s="9"/>
+      <c r="G71" s="10"/>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A72" s="9"/>
+      <c r="G72" s="10"/>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A73" s="9"/>
+      <c r="G73" s="10"/>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A74" s="9"/>
+      <c r="G74" s="10"/>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A75" s="9"/>
+      <c r="G75" s="18"/>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A76" s="9"/>
+      <c r="G76" s="18"/>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A77" s="9"/>
+      <c r="G77" s="10"/>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A78" s="9"/>
+      <c r="G78" s="19"/>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A79" s="9"/>
+      <c r="G79" s="10"/>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A80" s="9"/>
+      <c r="G80" s="10"/>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A81" s="9"/>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A82" s="9"/>
+      <c r="G82" s="10"/>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A83" s="9"/>
+      <c r="G83" s="10"/>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A84" s="9"/>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A85" s="9"/>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A86" s="9"/>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A88" s="9"/>
+      <c r="G88" s="10"/>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A89" s="9"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A90" s="9"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A91" s="9"/>
+      <c r="G91" s="10"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A92" s="9"/>
+      <c r="G92" s="10"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" s="9"/>
+      <c r="G93" s="10"/>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A94" s="9"/>
+      <c r="G94" s="10"/>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A95" s="9"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H19"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
pred sums of predictions by sale
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -22,7 +22,6 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">SCO!$A$1:$M$5</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="269">
   <si>
     <t>No</t>
   </si>
@@ -1135,9 +1134,6 @@
     <t>more pics (sco_v3)</t>
   </si>
   <si>
-    <t>last</t>
-  </si>
-  <si>
     <t>If early stopping condition is not encountered, weights are not reverted to best epoch's. Do more epochs</t>
   </si>
   <si>
@@ -1213,19 +1209,32 @@
   </si>
   <si>
     <t>Looks like 8 frames was optimum for top1</t>
+  </si>
+  <si>
+    <t>7 frames, but fixed issue splitting same sale to train/val</t>
+  </si>
+  <si>
+    <t>10 frame acc best</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="186"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1389,8 +1398,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -1400,13 +1409,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1436,20 +1448,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4712,7 +4721,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L21" sqref="L21"/>
+      <selection pane="bottomLeft" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4880,6 +4889,9 @@
       <c r="B6" s="7">
         <v>201</v>
       </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
       <c r="E6" s="6" t="s">
         <v>239</v>
       </c>
@@ -4906,6 +4918,9 @@
       <c r="B7" s="7">
         <v>202</v>
       </c>
+      <c r="C7" s="7">
+        <v>2</v>
+      </c>
       <c r="E7" s="6" t="s">
         <v>241</v>
       </c>
@@ -4922,7 +4937,7 @@
         <v>98.5</v>
       </c>
       <c r="L7" s="7" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -4930,8 +4945,11 @@
       <c r="B8" s="7">
         <v>202</v>
       </c>
+      <c r="C8" s="7">
+        <v>3</v>
+      </c>
       <c r="E8" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G8" s="5">
         <v>10</v>
@@ -4949,7 +4967,7 @@
         <v>98.7</v>
       </c>
       <c r="M8" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -4959,8 +4977,11 @@
       <c r="B9" s="7">
         <v>202</v>
       </c>
+      <c r="C9" s="7">
+        <v>4</v>
+      </c>
       <c r="E9" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="G9" s="5">
         <v>5</v>
@@ -4978,10 +4999,10 @@
         <v>98.2</v>
       </c>
       <c r="L9" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="M9" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="45" x14ac:dyDescent="0.25">
@@ -4991,8 +5012,11 @@
       <c r="B10" s="7">
         <v>202</v>
       </c>
+      <c r="C10" s="7">
+        <v>5</v>
+      </c>
       <c r="E10" s="6" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G10" s="5">
         <v>1</v>
@@ -5010,10 +5034,10 @@
         <v>99.1</v>
       </c>
       <c r="L10" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -5023,10 +5047,12 @@
       <c r="B11" s="23">
         <v>202</v>
       </c>
-      <c r="C11" s="23"/>
+      <c r="C11" s="7">
+        <v>6</v>
+      </c>
       <c r="D11" s="23"/>
       <c r="E11" s="24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G11" s="5">
         <v>3</v>
@@ -5044,7 +5070,7 @@
         <v>99.9</v>
       </c>
       <c r="L11" s="23" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -5054,10 +5080,12 @@
       <c r="B12" s="23">
         <v>202</v>
       </c>
-      <c r="C12" s="23"/>
+      <c r="C12" s="7">
+        <v>7</v>
+      </c>
       <c r="D12" s="23"/>
       <c r="E12" s="24" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H12" s="23">
         <v>49</v>
@@ -5072,7 +5100,7 @@
         <v>99.5</v>
       </c>
       <c r="L12" s="23" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
@@ -5082,10 +5110,12 @@
       <c r="B13" s="23">
         <v>202</v>
       </c>
-      <c r="C13" s="23"/>
+      <c r="C13" s="7">
+        <v>8</v>
+      </c>
       <c r="D13" s="23"/>
       <c r="E13" s="24" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H13" s="23">
         <v>55</v>
@@ -5100,7 +5130,7 @@
         <v>99.8</v>
       </c>
       <c r="L13" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
@@ -5110,10 +5140,12 @@
       <c r="B14" s="23">
         <v>202</v>
       </c>
-      <c r="C14" s="23"/>
+      <c r="C14" s="7">
+        <v>9</v>
+      </c>
       <c r="D14" s="23"/>
       <c r="E14" s="24" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G14" s="5">
         <v>2</v>
@@ -5131,7 +5163,7 @@
         <v>99.8</v>
       </c>
       <c r="L14" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
@@ -5141,10 +5173,12 @@
       <c r="B15" s="23">
         <v>202</v>
       </c>
-      <c r="C15" s="23"/>
+      <c r="C15" s="7">
+        <v>10</v>
+      </c>
       <c r="D15" s="23"/>
       <c r="E15" s="24" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H15" s="23">
         <v>61</v>
@@ -5159,7 +5193,7 @@
         <v>99.6</v>
       </c>
       <c r="L15" s="23" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -5169,12 +5203,12 @@
       <c r="B16" s="23">
         <v>202</v>
       </c>
-      <c r="C16" s="23" t="s">
-        <v>242</v>
+      <c r="C16" s="7">
+        <v>11</v>
       </c>
       <c r="D16" s="23"/>
       <c r="E16" s="24" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H16" s="23">
         <v>44</v>
@@ -5189,7 +5223,7 @@
         <v>98.8</v>
       </c>
       <c r="L16" s="23" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
@@ -5199,10 +5233,12 @@
       <c r="B17" s="23">
         <v>202</v>
       </c>
-      <c r="C17" s="23"/>
+      <c r="C17" s="7">
+        <v>12</v>
+      </c>
       <c r="D17" s="23"/>
       <c r="E17" s="24" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H17" s="23">
         <v>44</v>
@@ -5217,7 +5253,7 @@
         <v>98.9</v>
       </c>
       <c r="L17" s="23" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="30" x14ac:dyDescent="0.25">
@@ -5227,8 +5263,11 @@
       <c r="B18" s="7">
         <v>202</v>
       </c>
+      <c r="C18" s="7">
+        <v>13</v>
+      </c>
       <c r="E18" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G18" s="5">
         <v>3</v>
@@ -5253,8 +5292,11 @@
       <c r="B19" s="7">
         <v>202</v>
       </c>
+      <c r="C19" s="7">
+        <v>14</v>
+      </c>
       <c r="E19" s="6" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G19" s="5">
         <v>3</v>
@@ -5279,8 +5321,11 @@
       <c r="B20" s="7">
         <v>202</v>
       </c>
+      <c r="C20" s="7">
+        <v>15</v>
+      </c>
       <c r="E20" s="6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G20" s="5">
         <v>3</v>
@@ -5298,18 +5343,40 @@
         <v>97.6</v>
       </c>
       <c r="L20" s="7" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>43668</v>
+      </c>
+      <c r="B21" s="7">
+        <v>202</v>
+      </c>
+      <c r="C21" s="7">
+        <v>16</v>
+      </c>
+      <c r="E21" s="6" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
       <c r="G21" s="5">
         <v>3</v>
       </c>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
+      <c r="H21" s="25">
+        <v>48</v>
+      </c>
+      <c r="I21" s="25">
+        <v>99.8</v>
+      </c>
+      <c r="J21" s="25">
+        <v>81.5</v>
+      </c>
+      <c r="K21" s="25">
+        <v>97.3</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>

</xml_diff>